<commit_message>
Made changes to FHQ and Fanconi after EO updates
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/FHQScenario1.xlsx
+++ b/src/test/java/CHARMS/resources/FHQScenario1.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CCB7FC-6E05-D442-B559-AD39BB34544D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D44E6A-A7C2-F543-BD4A-529A3E38F136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="760" windowWidth="28620" windowHeight="17580" activeTab="7" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
+    <workbookView xWindow="1620" yWindow="760" windowWidth="28620" windowHeight="17580" activeTab="1" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
   </bookViews>
   <sheets>
-    <sheet name="Participant" sheetId="4" r:id="rId1"/>
-    <sheet name="Partner" sheetId="2" r:id="rId2"/>
-    <sheet name="Mother" sheetId="27" r:id="rId3"/>
-    <sheet name="Father" sheetId="26" r:id="rId4"/>
-    <sheet name="Children" sheetId="14" r:id="rId5"/>
-    <sheet name="Sibling" sheetId="29" r:id="rId6"/>
-    <sheet name="Aunt" sheetId="30" r:id="rId7"/>
-    <sheet name="Uncle" sheetId="17" r:id="rId8"/>
-    <sheet name="NieceNephew" sheetId="18" r:id="rId9"/>
-    <sheet name="MaternalGrandMother" sheetId="19" r:id="rId10"/>
-    <sheet name="MaternalGrandFather" sheetId="25" r:id="rId11"/>
-    <sheet name="PaternalGrandMother" sheetId="23" r:id="rId12"/>
-    <sheet name="PaternalGrandFather" sheetId="24" r:id="rId13"/>
-    <sheet name="GrandChildren" sheetId="21" r:id="rId14"/>
-    <sheet name="Cousin" sheetId="22" r:id="rId15"/>
-    <sheet name="Parent" sheetId="13" r:id="rId16"/>
+    <sheet name="RASScreener" sheetId="31" r:id="rId1"/>
+    <sheet name="Participant" sheetId="4" r:id="rId2"/>
+    <sheet name="Partner" sheetId="2" r:id="rId3"/>
+    <sheet name="Mother" sheetId="27" r:id="rId4"/>
+    <sheet name="Father" sheetId="26" r:id="rId5"/>
+    <sheet name="Children" sheetId="14" r:id="rId6"/>
+    <sheet name="Sibling" sheetId="29" r:id="rId7"/>
+    <sheet name="Aunt" sheetId="30" r:id="rId8"/>
+    <sheet name="Uncle" sheetId="17" r:id="rId9"/>
+    <sheet name="NieceNephew" sheetId="18" r:id="rId10"/>
+    <sheet name="MaternalGrandMother" sheetId="19" r:id="rId11"/>
+    <sheet name="MaternalGrandFather" sheetId="25" r:id="rId12"/>
+    <sheet name="PaternalGrandMother" sheetId="23" r:id="rId13"/>
+    <sheet name="PaternalGrandFather" sheetId="24" r:id="rId14"/>
+    <sheet name="GrandChildren" sheetId="21" r:id="rId15"/>
+    <sheet name="Cousin" sheetId="22" r:id="rId16"/>
+    <sheet name="Parent" sheetId="13" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sibling!$A$1:$B$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sibling!$A$1:$B$117</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3624" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3693" uniqueCount="528">
   <si>
     <t>Question</t>
   </si>
@@ -1467,13 +1468,187 @@
   </si>
   <si>
     <t>A partner I have reported in this questionnaire</t>
+  </si>
+  <si>
+    <t>Are you completing this form for someone else or for yourself?</t>
+  </si>
+  <si>
+    <t>I am completing this form for myself</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>DiegoFirstTest</t>
+  </si>
+  <si>
+    <t>Middle Initial</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>JuarezTest</t>
+  </si>
+  <si>
+    <t>What is your date of birth?</t>
+  </si>
+  <si>
+    <t>October 1, 1990</t>
+  </si>
+  <si>
+    <t>Date of birth month</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>Date of birth year</t>
+  </si>
+  <si>
+    <t>What was your sex assigned at birth?</t>
+  </si>
+  <si>
+    <t>Are you adopted?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>In which country do you currently live?</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Please provide the mailing address where study materials can be sent, as needed.</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>12-34 home address</t>
+  </si>
+  <si>
+    <t>Street 2 (optional)</t>
+  </si>
+  <si>
+    <t>Apt 600</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Burke</t>
+  </si>
+  <si>
+    <t>State (Abbreviation)</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>What is your email address?</t>
+  </si>
+  <si>
+    <t>charmsras1@yahoo.com</t>
+  </si>
+  <si>
+    <t>Please confirm your email address</t>
+  </si>
+  <si>
+    <t>Home phone number</t>
+  </si>
+  <si>
+    <t>703-687-5816</t>
+  </si>
+  <si>
+    <t>Cell phone number</t>
+  </si>
+  <si>
+    <t>703-687-5815</t>
+  </si>
+  <si>
+    <t>Work phone number</t>
+  </si>
+  <si>
+    <t>703-687-5814</t>
+  </si>
+  <si>
+    <t>What is your ethnicity?</t>
+  </si>
+  <si>
+    <t>Not Hispanic/Latino</t>
+  </si>
+  <si>
+    <t>What is your race? Please select all that apply.</t>
+  </si>
+  <si>
+    <t>Prefer not to answer</t>
+  </si>
+  <si>
+    <t>Are you a participant in any other research study or registry group?  Please specify.</t>
+  </si>
+  <si>
+    <t>I am not involved in any other research study or registry group</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with the following conditions?  Select all that apply.  If you do not see the exact condition diagnosed, please select the closest answer.</t>
+  </si>
+  <si>
+    <t>Never diagnosed with any of these conditions</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with cancer?</t>
+  </si>
+  <si>
+    <t>Have you been diagnosed with a RASopathy such as Noonan syndrome, Noonan syndrome with multiple lentigines, Costello syndrome, cardiofaciocutaneous syndrome, Legius syndrome, capillary arteriovenous malformation syndrome, hereditary gingival fibromatosis or SYNGAP1 syndrome?</t>
+  </si>
+  <si>
+    <t>Have any of your biological relatives been diagnosed with a RASopathy?</t>
+  </si>
+  <si>
+    <t>Have you ever had genetic testing?</t>
+  </si>
+  <si>
+    <t>How did you hear about this study?  If a specific health care provider referred you to this study, please include their name in the corresponding text box.</t>
+  </si>
+  <si>
+    <t>How did you hear about this study?  If a specific health care provider referred you to this study, please include their name in the corresponding text box. Other reason</t>
+  </si>
+  <si>
+    <t>JUST TESTING</t>
+  </si>
+  <si>
+    <t>Have you or other family members ever participated in another study on RASopathies at another medical institution, university, government agency or other site?</t>
+  </si>
+  <si>
+    <t>What are the main reasons for participating in this study?  Select all that apply.  Please elaborate on the reason in the corresponding textbox.</t>
+  </si>
+  <si>
+    <t>What are the main reasons for participating in this study?  Select all that apply.  Please elaborate on the reason in the corresponding textbox. Other reason</t>
+  </si>
+  <si>
+    <t>TESTING REASONS</t>
+  </si>
+  <si>
+    <t>You are almost done!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are almost done!
+  To submit your responses, you must continue in the questionnaire by clicking the forward arrow below.  
+The information you have provided will be reviewed by our study team.  If it is determined that you are eligible to participate in the RASopathy Study, you will receive an email with further details, including instructions to log in to a secure study portal. If the team decides that you are not eligible, you will receive an email explaining why. In the meantime, you should receive an email confirming this submission.
+  Please feel free to call at any time if you have any questions regarding this protocol and ask to speak with the RASopathies Study nurse. Our toll-free phone number is 1-800-518-8474 or 301-212-5250. Thank you for your willingness to consider joining our research effort.  We could not do vital studies like this without the help of dedicated patients and families.  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1515,6 +1690,22 @@
       <color theme="1"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1566,10 +1757,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1608,8 +1800,28 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1921,29 +2133,336 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4643CA46-B48D-824B-9B26-B5758EEE61DC}">
-  <dimension ref="A1:B73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451989A1-8DD1-7243-9E90-92372193E921}">
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="98.5" customWidth="1"/>
+    <col min="2" max="2" width="53" style="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>476</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>478</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>480</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>483</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>486</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>489</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="B17" s="17">
+        <v>22015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>498</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>507</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>511</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>513</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>516</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>518</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>520</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="16" t="s">
+        <v>522</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>524</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="323" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>527</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B18" r:id="rId1" xr:uid="{B707E8B0-A2C9-1045-B029-4439D6A8416A}"/>
+    <hyperlink ref="B19" r:id="rId2" xr:uid="{53EA57A8-FDBD-8B4A-9A69-4E062F90D3A8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C165AD-8F20-F342-8EE0-C1843FC10E3A}">
+  <dimension ref="A1:D128"/>
+  <sheetViews>
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="88" style="3" customWidth="1"/>
-    <col min="2" max="2" width="119.6640625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="69.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="102.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="22" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="22" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1951,572 +2470,995 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="66" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="44" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="88" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>424</v>
+        <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="66" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="22" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>425</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="22" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>426</v>
+        <v>72</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="22" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>255</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="22" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>256</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="44" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="22" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>205</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" ht="22" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>257</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>428</v>
+        <v>71</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>10</v>
+        <v>207</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>12</v>
+        <v>258</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>13</v>
+        <v>259</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>460</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>14</v>
+        <v>464</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>371</v>
+        <v>260</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>459</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>31</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>16</v>
+        <v>213</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>17</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>365</v>
+        <v>6</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>365</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>18</v>
+        <v>263</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>33</v>
+        <v>454</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>366</v>
+        <v>442</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>357</v>
+        <v>265</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1900</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B49" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B51" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="3" t="s">
+    <row r="52" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B71" s="3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B72" s="3"/>
+    </row>
+    <row r="73" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B82" s="3"/>
+    </row>
+    <row r="83" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B83" s="3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B92" s="3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B104" s="3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B105" s="3"/>
+    </row>
+    <row r="106" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B108" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="66" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="B109" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B111" s="3" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    <row r="112" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B112" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    <row r="113" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+    <row r="114" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B114" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+    <row r="115" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+    <row r="116" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+    <row r="117" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="B117" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="B118" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+    <row r="120" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B120" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B56" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
+    <row r="121" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
+      <c r="B123" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B125" s="3" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>461</v>
+    <row r="126" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A126" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A127" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2524,7 +3466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9316003E-8C1B-C646-9C81-76A5577493AC}">
   <dimension ref="A1:D131"/>
   <sheetViews>
@@ -3552,7 +4494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E1A8D1-EF16-614B-9787-207F67568443}">
   <dimension ref="A1:B131"/>
   <sheetViews>
@@ -4583,7 +5525,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4481BEE8-084A-6544-B91F-4F54426F0338}">
   <dimension ref="A1:B131"/>
   <sheetViews>
@@ -5608,7 +6550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FE5151-D152-9D4A-B20B-CB625C7763F4}">
   <dimension ref="A1:B131"/>
   <sheetViews>
@@ -6655,7 +7597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200F2574-0F76-5848-B5CA-B19DBB029645}">
   <dimension ref="A1:D122"/>
   <sheetViews>
@@ -7634,7 +8576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90F0027-F00B-1B4B-AE3D-053640C4AD50}">
   <dimension ref="A1:D135"/>
   <sheetViews>
@@ -8715,7 +9657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{686FEE5D-0F02-AC40-AA06-77804C89CACF}">
   <dimension ref="A1:B135"/>
   <sheetViews>
@@ -9775,6 +10717,610 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4643CA46-B48D-824B-9B26-B5758EEE61DC}">
+  <dimension ref="A1:B73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="88" style="3" customWidth="1"/>
+    <col min="2" max="2" width="119.6640625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="66" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="88" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="66" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>461</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD80803-AE11-A144-B3B5-0F8781481FD1}">
   <dimension ref="A1:B45"/>
   <sheetViews>
@@ -10151,7 +11697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DE6941-7806-3846-9E89-FFA2416775F2}">
   <dimension ref="A1:B131"/>
   <sheetViews>
@@ -11176,7 +12722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DAC041-37A0-CC45-933E-8E0EC3CE87DA}">
   <dimension ref="A1:B132"/>
   <sheetViews>
@@ -12221,7 +13767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3F8D73-A2F8-A34D-BAA9-8CA076BBD188}">
   <dimension ref="A1:B140"/>
   <sheetViews>
@@ -13342,7 +14888,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF2E6C6-AC83-AD43-B24B-8118763EC5A4}">
   <dimension ref="A1:B117"/>
   <sheetViews>
@@ -14282,7 +15828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D440C8FC-FCC1-A240-91E3-288B715C9C66}">
   <dimension ref="A1:B134"/>
   <sheetViews>
@@ -15348,11 +16894,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A1A7AA-D469-814C-86B3-A8D7D6B424B5}">
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -16419,1030 +17965,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C165AD-8F20-F342-8EE0-C1843FC10E3A}">
-  <dimension ref="A1:D128"/>
-  <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="69.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="102.6640625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="44" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="44" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="66" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="66" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B48" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B51" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B71" s="3">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B83" s="3">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="B92" s="3">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B104" s="3">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B105" s="3"/>
-    </row>
-    <row r="106" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A106" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A108" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B108" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="66" x14ac:dyDescent="0.2">
-      <c r="A109" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A115" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A117" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A118" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A119" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A120" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A121" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A122" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A123" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A124" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A125" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A126" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A127" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A128" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Fanconi and FHQ test cases based on new updates
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/FHQScenario1.xlsx
+++ b/src/test/java/CHARMS/resources/FHQScenario1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D44E6A-A7C2-F543-BD4A-529A3E38F136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4604DA1-F7C2-984E-9CA1-029A99A0DA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="760" windowWidth="28620" windowHeight="17580" activeTab="1" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
+    <workbookView xWindow="1620" yWindow="760" windowWidth="28620" windowHeight="17580" activeTab="2" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
   </bookViews>
   <sheets>
     <sheet name="RASScreener" sheetId="31" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3693" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3693" uniqueCount="529">
   <si>
     <t>Question</t>
   </si>
@@ -1642,6 +1642,9 @@
   To submit your responses, you must continue in the questionnaire by clicking the forward arrow below.  
 The information you have provided will be reviewed by our study team.  If it is determined that you are eligible to participate in the RASopathy Study, you will receive an email with further details, including instructions to log in to a secure study portal. If the team decides that you are not eligible, you will receive an email explaining why. In the meantime, you should receive an email confirming this submission.
   Please feel free to call at any time if you have any questions regarding this protocol and ask to speak with the RASopathies Study nurse. Our toll-free phone number is 1-800-518-8474 or 301-212-5250. Thank you for your willingness to consider joining our research effort.  We could not do vital studies like this without the help of dedicated patients and families.  </t>
+  </si>
+  <si>
+    <t>Sex</t>
   </si>
 </sst>
 </file>
@@ -10720,8 +10723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4643CA46-B48D-824B-9B26-B5758EEE61DC}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -10909,7 +10912,7 @@
     </row>
     <row r="23" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>15</v>
+        <v>528</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>31</v>
@@ -11324,8 +11327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD80803-AE11-A144-B3B5-0F8781481FD1}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11561,7 +11564,7 @@
         <v>15</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>15</v>
+        <v>528</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -11701,8 +11704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DE6941-7806-3846-9E89-FFA2416775F2}">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD49"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -12004,7 +12007,7 @@
         <v>15</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>15</v>
+        <v>528</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -12727,7 +12730,7 @@
   <dimension ref="A1:B132"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD49"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -13041,7 +13044,7 @@
         <v>15</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>15</v>
+        <v>528</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13771,7 +13774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3F8D73-A2F8-A34D-BAA9-8CA076BBD188}">
   <dimension ref="A1:B140"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated  Fanconi and FHQ scripts after enhancement
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/FHQScenario1.xlsx
+++ b/src/test/java/CHARMS/resources/FHQScenario1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4604DA1-F7C2-984E-9CA1-029A99A0DA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55DCF1C-2ADC-4F4B-AF2D-D67A3A46ED6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="760" windowWidth="28620" windowHeight="17580" activeTab="2" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
+    <workbookView xWindow="16120" yWindow="500" windowWidth="35080" windowHeight="17580" firstSheet="1" activeTab="7" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
   </bookViews>
   <sheets>
     <sheet name="RASScreener" sheetId="31" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <sheet name="Parent" sheetId="13" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sibling!$A$1:$B$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sibling!$A$1:$B$118</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3693" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3695" uniqueCount="529">
   <si>
     <t>Question</t>
   </si>
@@ -1195,9 +1195,6 @@
   </si>
   <si>
     <t>There is nothing else to mention about the Father</t>
-  </si>
-  <si>
-    <t>FHQ Patient: sonikatestaccount sonikatestaccount</t>
   </si>
   <si>
     <t>ParticipantAuntFirstName</t>
@@ -1645,6 +1642,9 @@
   </si>
   <si>
     <t>Sex</t>
+  </si>
+  <si>
+    <t>FHQ Patient: CHARMSRASopathy</t>
   </si>
 </sst>
 </file>
@@ -2159,23 +2159,23 @@
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
+        <v>470</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>471</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>473</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>233</v>
@@ -2183,31 +2183,31 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>476</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>478</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>480</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B8" s="17">
         <v>1990</v>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>31</v>
@@ -2223,60 +2223,60 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
+        <v>483</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>484</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
+        <v>485</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>486</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>489</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
+        <v>490</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>491</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
+        <v>492</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>493</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
+        <v>494</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>495</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B17" s="17">
         <v>22015</v>
@@ -2284,111 +2284,111 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>498</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>501</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
+        <v>502</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>503</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>505</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>507</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
+        <v>508</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>509</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
+        <v>510</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>511</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>513</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>91</v>
@@ -2396,23 +2396,23 @@
     </row>
     <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>520</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>91</v>
@@ -2420,18 +2420,18 @@
     </row>
     <row r="35" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>524</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="323" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="B36" s="20" t="s">
         <v>526</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -2447,8 +2447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C165AD-8F20-F342-8EE0-C1843FC10E3A}">
   <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A71" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:XFD86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -2526,7 +2526,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22" x14ac:dyDescent="0.2">
@@ -2624,7 +2624,7 @@
         <v>210</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -2671,10 +2671,10 @@
     </row>
     <row r="28" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -2695,7 +2695,7 @@
     </row>
     <row r="31" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>85</v>
@@ -2903,10 +2903,10 @@
     </row>
     <row r="57" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="58" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -3125,17 +3125,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>32</v>
@@ -3143,39 +3143,39 @@
     </row>
     <row r="88" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B92" s="3">
         <v>1900</v>
@@ -3183,15 +3183,15 @@
     </row>
     <row r="93" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="95" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -3306,10 +3306,10 @@
     </row>
     <row r="109" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -3322,10 +3322,10 @@
     </row>
     <row r="111" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="112" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -3426,18 +3426,18 @@
     </row>
     <row r="124" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -3473,8 +3473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9316003E-8C1B-C646-9C81-76A5577493AC}">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A88" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:XFD103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -3557,10 +3557,10 @@
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22" x14ac:dyDescent="0.2">
@@ -3826,7 +3826,7 @@
     </row>
     <row r="47" spans="1:3" s="5" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>85</v>
@@ -4034,10 +4034,10 @@
     </row>
     <row r="73" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="74" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -4264,17 +4264,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>32</v>
@@ -4282,39 +4282,39 @@
     </row>
     <row r="105" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B109" s="3">
         <v>1900</v>
@@ -4322,16 +4322,16 @@
     </row>
     <row r="110" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B110" s="3"/>
     </row>
     <row r="111" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="112" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -4449,23 +4449,23 @@
         <v>63</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -4501,8 +4501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E1A8D1-EF16-614B-9787-207F67568443}">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A89" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:XFD103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -4585,10 +4585,10 @@
     </row>
     <row r="10" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -4857,7 +4857,7 @@
     </row>
     <row r="47" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>85</v>
@@ -5065,10 +5065,10 @@
     </row>
     <row r="73" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -5295,17 +5295,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>32</v>
@@ -5313,39 +5313,39 @@
     </row>
     <row r="105" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B109" s="3">
         <v>1900</v>
@@ -5353,16 +5353,16 @@
     </row>
     <row r="110" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B110" s="3"/>
     </row>
     <row r="111" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -5485,18 +5485,18 @@
     </row>
     <row r="127" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -5532,8 +5532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4481BEE8-084A-6544-B91F-4F54426F0338}">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A91" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:XFD103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -5616,10 +5616,10 @@
     </row>
     <row r="10" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -5888,7 +5888,7 @@
     </row>
     <row r="47" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>85</v>
@@ -6096,10 +6096,10 @@
     </row>
     <row r="73" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -6322,17 +6322,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>32</v>
@@ -6340,39 +6340,39 @@
     </row>
     <row r="105" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B109" s="3">
         <v>1900</v>
@@ -6380,15 +6380,15 @@
     </row>
     <row r="110" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -6510,18 +6510,18 @@
     </row>
     <row r="127" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -6557,8 +6557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FE5151-D152-9D4A-B20B-CB625C7763F4}">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:XFD103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -6641,10 +6641,10 @@
     </row>
     <row r="10" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -6769,7 +6769,7 @@
     </row>
     <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>284</v>
@@ -6780,7 +6780,7 @@
         <v>327</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -6929,7 +6929,7 @@
     </row>
     <row r="47" spans="1:2" ht="88" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>85</v>
@@ -7137,10 +7137,10 @@
     </row>
     <row r="73" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -7367,17 +7367,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>32</v>
@@ -7385,39 +7385,39 @@
     </row>
     <row r="105" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B109" s="3">
         <v>1900</v>
@@ -7425,16 +7425,16 @@
     </row>
     <row r="110" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B110" s="3"/>
     </row>
     <row r="111" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="66" x14ac:dyDescent="0.2">
@@ -7557,18 +7557,18 @@
     </row>
     <row r="127" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -7604,8 +7604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200F2574-0F76-5848-B5CA-B19DBB029645}">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:XFD91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -7688,10 +7688,10 @@
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22" x14ac:dyDescent="0.2">
@@ -7789,7 +7789,7 @@
         <v>210</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -7837,10 +7837,10 @@
     </row>
     <row r="29" spans="1:2" ht="88" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -7877,10 +7877,10 @@
     </row>
     <row r="34" spans="1:2" s="7" customFormat="1" ht="110" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -8101,10 +8101,10 @@
     </row>
     <row r="62" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="63" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -8323,17 +8323,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>32</v>
@@ -8341,39 +8341,39 @@
     </row>
     <row r="93" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B97" s="3">
         <v>1900</v>
@@ -8381,15 +8381,15 @@
     </row>
     <row r="98" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="100" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -8496,10 +8496,10 @@
     </row>
     <row r="113" spans="1:2" ht="88" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -8536,18 +8536,18 @@
     </row>
     <row r="118" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -8583,8 +8583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90F0027-F00B-1B4B-AE3D-053640C4AD50}">
   <dimension ref="A1:D135"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -8659,10 +8659,10 @@
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22" x14ac:dyDescent="0.2">
@@ -8744,7 +8744,7 @@
         <v>346</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -8757,10 +8757,10 @@
     </row>
     <row r="21" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -8787,7 +8787,7 @@
     </row>
     <row r="25" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B25" s="3"/>
     </row>
@@ -8796,7 +8796,7 @@
         <v>334</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -8804,15 +8804,15 @@
         <v>335</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -8831,7 +8831,7 @@
     </row>
     <row r="31" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>310</v>
@@ -8839,7 +8839,7 @@
     </row>
     <row r="32" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B32" s="3"/>
     </row>
@@ -8848,7 +8848,7 @@
         <v>275</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -8864,7 +8864,7 @@
         <v>210</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -8917,10 +8917,10 @@
     </row>
     <row r="42" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>445</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -8944,7 +8944,7 @@
         <v>287</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -8957,7 +8957,7 @@
     </row>
     <row r="47" spans="1:2" s="7" customFormat="1" ht="66" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>85</v>
@@ -9181,10 +9181,10 @@
     </row>
     <row r="75" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="76" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -9403,17 +9403,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>32</v>
@@ -9421,39 +9421,39 @@
     </row>
     <row r="106" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B110" s="3">
         <v>1900</v>
@@ -9461,16 +9461,16 @@
     </row>
     <row r="111" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B111" s="3"/>
     </row>
     <row r="112" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B112" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="113" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -9577,10 +9577,10 @@
     </row>
     <row r="126" spans="1:2" ht="88" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -9617,18 +9617,18 @@
     </row>
     <row r="131" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -9949,7 +9949,7 @@
     </row>
     <row r="38" spans="1:2" ht="88" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>85</v>
@@ -10197,10 +10197,10 @@
     </row>
     <row r="69" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -10393,15 +10393,15 @@
     </row>
     <row r="95" spans="1:2" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="96" spans="1:2" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>32</v>
@@ -10409,39 +10409,39 @@
     </row>
     <row r="97" spans="1:2" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="98" spans="1:2" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="99" spans="1:2" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="100" spans="1:2" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="101" spans="1:2" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B101" s="3">
         <v>1900</v>
@@ -10449,16 +10449,16 @@
     </row>
     <row r="102" spans="1:2" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B102" s="3"/>
     </row>
     <row r="103" spans="1:2" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B103" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -10676,18 +10676,18 @@
     </row>
     <row r="131" spans="1:2" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="132" spans="1:2" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="133" spans="1:2" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -10723,7 +10723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4643CA46-B48D-824B-9B26-B5758EEE61DC}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -10755,31 +10755,31 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="88" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -10824,10 +10824,10 @@
     </row>
     <row r="12" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -10891,7 +10891,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -10907,12 +10907,12 @@
         <v>371</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>31</v>
@@ -11027,7 +11027,7 @@
         <v>24</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -11040,10 +11040,10 @@
     </row>
     <row r="39" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -11184,10 +11184,10 @@
     </row>
     <row r="57" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -11280,18 +11280,18 @@
     </row>
     <row r="69" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -11315,7 +11315,7 @@
         <v>373</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -11327,8 +11327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD80803-AE11-A144-B3B5-0F8781481FD1}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11411,10 +11411,10 @@
     </row>
     <row r="10" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -11492,7 +11492,7 @@
         <v>104</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -11545,7 +11545,7 @@
     </row>
     <row r="27" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>85</v>
@@ -11564,7 +11564,7 @@
         <v>15</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -11657,18 +11657,18 @@
     </row>
     <row r="41" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -11704,8 +11704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DE6941-7806-3846-9E89-FFA2416775F2}">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -11788,10 +11788,10 @@
     </row>
     <row r="10" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -11900,7 +11900,7 @@
     </row>
     <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>105</v>
@@ -11980,7 +11980,7 @@
     </row>
     <row r="37" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>85</v>
@@ -12004,10 +12004,10 @@
     </row>
     <row r="40" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>15</v>
+        <v>527</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -12180,10 +12180,10 @@
     </row>
     <row r="62" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -12408,15 +12408,15 @@
     </row>
     <row r="92" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>32</v>
@@ -12424,31 +12424,31 @@
     </row>
     <row r="94" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B97" s="3">
         <v>1900</v>
@@ -12456,15 +12456,15 @@
     </row>
     <row r="98" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -12573,7 +12573,7 @@
         <v>148</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -12629,7 +12629,7 @@
         <v>194</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -12637,7 +12637,7 @@
         <v>197</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -12682,18 +12682,18 @@
     </row>
     <row r="127" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -12729,8 +12729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DAC041-37A0-CC45-933E-8E0EC3CE87DA}">
   <dimension ref="A1:B132"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -12813,10 +12813,10 @@
     </row>
     <row r="10" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -12937,7 +12937,7 @@
     </row>
     <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>280</v>
+        <v>449</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>105</v>
@@ -13017,7 +13017,7 @@
     </row>
     <row r="37" spans="1:2" ht="110" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>85</v>
@@ -13041,10 +13041,10 @@
     </row>
     <row r="40" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>15</v>
+        <v>527</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13217,10 +13217,10 @@
     </row>
     <row r="62" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13445,15 +13445,15 @@
     </row>
     <row r="92" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>32</v>
@@ -13461,39 +13461,39 @@
     </row>
     <row r="94" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B98" s="3">
         <v>1900</v>
@@ -13501,15 +13501,15 @@
     </row>
     <row r="99" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B100" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -13618,7 +13618,7 @@
         <v>148</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13658,7 +13658,7 @@
         <v>191</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13674,7 +13674,7 @@
         <v>194</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13682,7 +13682,7 @@
         <v>197</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13727,18 +13727,18 @@
     </row>
     <row r="128" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13774,8 +13774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3F8D73-A2F8-A34D-BAA9-8CA076BBD188}">
   <dimension ref="A1:B140"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:XFD104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -13858,10 +13858,10 @@
     </row>
     <row r="10" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13933,7 +13933,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>15</v>
+        <v>527</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -14005,10 +14005,10 @@
     </row>
     <row r="29" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>435</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -14029,7 +14029,7 @@
     </row>
     <row r="32" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>85</v>
@@ -14085,18 +14085,18 @@
     </row>
     <row r="39" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
@@ -14117,10 +14117,10 @@
     </row>
     <row r="43" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -14133,7 +14133,7 @@
     </row>
     <row r="45" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>361</v>
@@ -14293,10 +14293,10 @@
     </row>
     <row r="65" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="66" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -14523,17 +14523,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>32</v>
@@ -14541,39 +14541,39 @@
     </row>
     <row r="97" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B101" s="3">
         <v>1900</v>
@@ -14581,15 +14581,15 @@
     </row>
     <row r="102" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B103" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="104" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -14704,10 +14704,10 @@
     </row>
     <row r="118" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="119" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -14720,10 +14720,10 @@
     </row>
     <row r="120" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="121" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -14824,18 +14824,18 @@
     </row>
     <row r="133" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -14883,7 +14883,7 @@
         <v>210</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>380</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>
@@ -14893,10 +14893,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF2E6C6-AC83-AD43-B24B-8118763EC5A4}">
-  <dimension ref="A1:B117"/>
+  <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -14974,7 +14974,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -15096,7 +15096,7 @@
     </row>
     <row r="25" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>85</v>
@@ -15304,10 +15304,10 @@
     </row>
     <row r="51" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -15528,15 +15528,15 @@
     </row>
     <row r="80" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>32</v>
@@ -15544,39 +15544,39 @@
     </row>
     <row r="82" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B86" s="3">
         <v>1900</v>
@@ -15584,23 +15584,23 @@
     </row>
     <row r="87" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="89" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>144</v>
+        <v>462</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>144</v>
+        <v>462</v>
       </c>
     </row>
     <row r="90" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
@@ -15613,220 +15613,228 @@
     </row>
     <row r="91" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
     </row>
     <row r="92" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="95" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="96" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
     </row>
     <row r="97" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B98" s="3">
-        <v>1900</v>
+        <v>182</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="99" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B99" s="3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B99" s="3"/>
-    </row>
-    <row r="100" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
+      <c r="B100" s="3"/>
+    </row>
+    <row r="101" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="101" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
+    <row r="102" spans="1:2" s="1" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
+    <row r="103" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B102" s="3">
+      <c r="B103" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="88" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" ht="88" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="22" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>419</v>
+        <v>438</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>419</v>
+        <v>438</v>
       </c>
     </row>
     <row r="107" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>39</v>
+        <v>418</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>244</v>
+        <v>418</v>
       </c>
     </row>
     <row r="108" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B110" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
+    <row r="111" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B111" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="111" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
+    <row r="112" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B112" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="112" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
+    <row r="113" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="44" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>374</v>
+        <v>417</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>374</v>
+        <v>417</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="22" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>320</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B117" xr:uid="{FEF2E6C6-AC83-AD43-B24B-8118763EC5A4}"/>
+  <autoFilter ref="A1:B118" xr:uid="{FEF2E6C6-AC83-AD43-B24B-8118763EC5A4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -15835,8 +15843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D440C8FC-FCC1-A240-91E3-288B715C9C66}">
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -15914,7 +15922,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -15959,23 +15967,23 @@
     </row>
     <row r="15" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>38</v>
@@ -15983,7 +15991,7 @@
     </row>
     <row r="18" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -15993,23 +16001,23 @@
     </row>
     <row r="20" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>38</v>
@@ -16017,7 +16025,7 @@
     </row>
     <row r="23" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -16027,23 +16035,23 @@
     </row>
     <row r="25" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>38</v>
@@ -16075,10 +16083,10 @@
     </row>
     <row r="31" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -16099,7 +16107,7 @@
     </row>
     <row r="34" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>85</v>
@@ -16307,10 +16315,10 @@
     </row>
     <row r="60" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="61" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -16529,17 +16537,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>32</v>
@@ -16547,39 +16555,39 @@
     </row>
     <row r="91" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B95" s="3">
         <v>1900</v>
@@ -16587,15 +16595,15 @@
     </row>
     <row r="96" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="98" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -16710,10 +16718,10 @@
     </row>
     <row r="112" spans="1:2" ht="88" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="113" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -16726,10 +16734,10 @@
     </row>
     <row r="114" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="115" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -16777,7 +16785,7 @@
         <v>39</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="121" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -16785,7 +16793,7 @@
         <v>40</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="122" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -16825,23 +16833,23 @@
         <v>63</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -16870,23 +16878,23 @@
     </row>
     <row r="132" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B132" s="3" t="s">
         <v>394</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>58</v>
@@ -16901,8 +16909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A1A7AA-D469-814C-86B3-A8D7D6B424B5}">
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -16980,7 +16988,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -17025,24 +17033,24 @@
     </row>
     <row r="15" spans="1:3" ht="22" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" ht="22" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>38</v>
@@ -17050,7 +17058,7 @@
     </row>
     <row r="18" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>320</v>
@@ -17061,28 +17069,28 @@
         <v>279</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>38</v>
@@ -17090,7 +17098,7 @@
     </row>
     <row r="23" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -17100,23 +17108,23 @@
     </row>
     <row r="25" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>38</v>
@@ -17148,10 +17156,10 @@
     </row>
     <row r="31" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -17172,7 +17180,7 @@
     </row>
     <row r="34" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>85</v>
@@ -17247,7 +17255,7 @@
         <v>131</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -17380,10 +17388,10 @@
     </row>
     <row r="60" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="61" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -17602,17 +17610,17 @@
         <v>187</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>32</v>
@@ -17620,39 +17628,39 @@
     </row>
     <row r="91" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B95" s="3">
         <v>1900</v>
@@ -17660,15 +17668,15 @@
     </row>
     <row r="96" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="98" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -17783,10 +17791,10 @@
     </row>
     <row r="112" spans="1:2" ht="88" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="113" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -17799,10 +17807,10 @@
     </row>
     <row r="114" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="115" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -17850,7 +17858,7 @@
         <v>39</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="121" spans="1:2" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -17898,23 +17906,23 @@
         <v>63</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="44" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -17943,23 +17951,23 @@
     </row>
     <row r="132" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B132" s="3" t="s">
         <v>394</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
changed made in FHQ and Fanconi based on the new enhancements
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/FHQScenario1.xlsx
+++ b/src/test/java/CHARMS/resources/FHQScenario1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55DCF1C-2ADC-4F4B-AF2D-D67A3A46ED6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D4AF11-F1E5-CD4F-83FD-9B7C139520A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16120" yWindow="500" windowWidth="35080" windowHeight="17580" firstSheet="1" activeTab="7" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" firstSheet="1" activeTab="12" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
   </bookViews>
   <sheets>
     <sheet name="RASScreener" sheetId="31" r:id="rId1"/>
@@ -1446,9 +1446,6 @@
     <t>Has this relative ever been diagnosed with one of the benign tumors listed below?</t>
   </si>
   <si>
-    <t>FHQ Siblings: ParticipantSiblingFirstName</t>
-  </si>
-  <si>
     <t>FHQ Aunt/Uncle: ParticipantUncleFirstName</t>
   </si>
   <si>
@@ -1645,6 +1642,9 @@
   </si>
   <si>
     <t>FHQ Patient: CHARMSRASopathy</t>
+  </si>
+  <si>
+    <t>FHQ Siblings: ParticipantSiblingFirstNam...</t>
   </si>
 </sst>
 </file>
@@ -2159,23 +2159,23 @@
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>470</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>472</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>233</v>
@@ -2183,31 +2183,31 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
+        <v>474</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>475</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>476</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>477</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
+        <v>478</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>479</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B8" s="17">
         <v>1990</v>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>31</v>
@@ -2223,60 +2223,60 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>483</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>485</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
+        <v>487</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>488</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
+        <v>489</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>490</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>492</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>494</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B17" s="17">
         <v>22015</v>
@@ -2284,111 +2284,111 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>497</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
+        <v>499</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>500</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>502</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>504</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>506</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>510</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
+        <v>511</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>512</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>91</v>
@@ -2396,23 +2396,23 @@
     </row>
     <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
+        <v>518</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>519</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>91</v>
@@ -2420,18 +2420,18 @@
     </row>
     <row r="35" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
+        <v>522</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>523</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="323" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
+        <v>524</v>
+      </c>
+      <c r="B36" s="20" t="s">
         <v>525</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -2447,8 +2447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C165AD-8F20-F342-8EE0-C1843FC10E3A}">
   <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86:XFD86"/>
+    <sheetView topLeftCell="A7" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -2597,10 +2597,10 @@
     </row>
     <row r="18" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>526</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>15</v>
+        <v>526</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -2624,7 +2624,7 @@
         <v>210</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>463</v>
+        <v>528</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -3473,8 +3473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9316003E-8C1B-C646-9C81-76A5577493AC}">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="75" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:XFD103"/>
+    <sheetView topLeftCell="A40" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -3853,7 +3853,7 @@
         <v>15</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>15</v>
+        <v>526</v>
       </c>
     </row>
     <row r="51" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -4501,8 +4501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E1A8D1-EF16-614B-9787-207F67568443}">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:XFD103"/>
+    <sheetView topLeftCell="A32" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -4884,7 +4884,7 @@
         <v>15</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>15</v>
+        <v>526</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -5532,8 +5532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4481BEE8-084A-6544-B91F-4F54426F0338}">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:XFD103"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -5915,7 +5915,7 @@
         <v>15</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>15</v>
+        <v>526</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -8864,7 +8864,7 @@
         <v>210</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -10912,7 +10912,7 @@
     </row>
     <row r="23" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>31</v>
@@ -11564,7 +11564,7 @@
         <v>15</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -12004,10 +12004,10 @@
     </row>
     <row r="40" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13041,10 +13041,10 @@
     </row>
     <row r="40" spans="1:2" ht="22" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13933,7 +13933,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -14085,18 +14085,18 @@
     </row>
     <row r="39" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="5" customFormat="1" ht="66" x14ac:dyDescent="0.2">
@@ -14117,10 +14117,10 @@
     </row>
     <row r="43" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
@@ -14133,7 +14133,7 @@
     </row>
     <row r="45" spans="1:2" s="5" customFormat="1" ht="44" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>361</v>
@@ -14883,7 +14883,7 @@
         <v>210</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -15843,7 +15843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D440C8FC-FCC1-A240-91E3-288B715C9C66}">
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made changes after the PR
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/FHQScenario1.xlsx
+++ b/src/test/java/CHARMS/resources/FHQScenario1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D4AF11-F1E5-CD4F-83FD-9B7C139520A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59724D35-64FF-4340-A288-AADEB28AA9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" firstSheet="1" activeTab="12" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" firstSheet="4" activeTab="14" xr2:uid="{0B804629-B76C-2342-A931-14829AE33D19}"/>
   </bookViews>
   <sheets>
     <sheet name="RASScreener" sheetId="31" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3695" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3695" uniqueCount="536">
   <si>
     <t>Question</t>
   </si>
@@ -1645,6 +1645,27 @@
   </si>
   <si>
     <t>FHQ Siblings: ParticipantSiblingFirstNam...</t>
+  </si>
+  <si>
+    <t>Atypical Spitz tumor</t>
+  </si>
+  <si>
+    <t>Cystic nephroma</t>
+  </si>
+  <si>
+    <t>Lipoma</t>
+  </si>
+  <si>
+    <t>Schwannoma</t>
+  </si>
+  <si>
+    <t>Spitz nevus</t>
+  </si>
+  <si>
+    <t>Giant congenital nevus</t>
+  </si>
+  <si>
+    <t>Neurofibroma</t>
   </si>
 </sst>
 </file>
@@ -2447,8 +2468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C165AD-8F20-F342-8EE0-C1843FC10E3A}">
   <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A73" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -3170,7 +3191,7 @@
         <v>412</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>432</v>
+        <v>534</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -3473,8 +3494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9316003E-8C1B-C646-9C81-76A5577493AC}">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView topLeftCell="A93" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -4309,7 +4330,7 @@
         <v>412</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>432</v>
+        <v>535</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -4501,8 +4522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E1A8D1-EF16-614B-9787-207F67568443}">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView topLeftCell="A46" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -5340,7 +5361,7 @@
         <v>412</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>432</v>
+        <v>530</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -5532,8 +5553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4481BEE8-084A-6544-B91F-4F54426F0338}">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A105" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -6367,7 +6388,7 @@
         <v>412</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>432</v>
+        <v>532</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -6399,7 +6420,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="44" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" ht="66" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>146</v>
       </c>
@@ -6558,7 +6579,7 @@
   <dimension ref="A1:B131"/>
   <sheetViews>
     <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:XFD103"/>
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -7412,7 +7433,7 @@
         <v>412</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>432</v>
+        <v>531</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="44" x14ac:dyDescent="0.2">
@@ -7604,8 +7625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200F2574-0F76-5848-B5CA-B19DBB029645}">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91:XFD91"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -7904,7 +7925,7 @@
         <v>15</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>15</v>
+        <v>526</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.2">
@@ -8368,7 +8389,7 @@
         <v>412</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>432</v>
+        <v>531</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -8583,8 +8604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90F0027-F00B-1B4B-AE3D-053640C4AD50}">
   <dimension ref="A1:D135"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -9448,7 +9469,7 @@
         <v>412</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>432</v>
+        <v>531</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -11704,8 +11725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DE6941-7806-3846-9E89-FFA2416775F2}">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -12443,7 +12464,7 @@
         <v>412</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>432</v>
+        <v>529</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -12729,8 +12750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DAC041-37A0-CC45-933E-8E0EC3CE87DA}">
   <dimension ref="A1:B132"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -13488,7 +13509,7 @@
         <v>412</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>432</v>
+        <v>530</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -13774,8 +13795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3F8D73-A2F8-A34D-BAA9-8CA076BBD188}">
   <dimension ref="A1:B140"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104:XFD104"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -14568,7 +14589,7 @@
         <v>412</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>432</v>
+        <v>531</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -14895,8 +14916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF2E6C6-AC83-AD43-B24B-8118763EC5A4}">
   <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:XFD89"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -15571,7 +15592,7 @@
         <v>412</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>432</v>
+        <v>532</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -15843,8 +15864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D440C8FC-FCC1-A240-91E3-288B715C9C66}">
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -16582,7 +16603,7 @@
         <v>412</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>432</v>
+        <v>533</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="22" x14ac:dyDescent="0.2">
@@ -16909,7 +16930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A1A7AA-D469-814C-86B3-A8D7D6B424B5}">
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>

</xml_diff>